<commit_message>
output Excel file style
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -26,12 +26,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00BEBEBE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFE0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B4EEB4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F0FFF0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,8 +66,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,134 +522,404 @@
           <t>赠送/直购</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr"/>
-      <c r="P1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>备注</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>王五</t>
+        </is>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>15935502580</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>王6</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>15935502580</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2" t="n"/>
+      <c r="G3" s="2" t="n"/>
+      <c r="H3" s="2" t="n"/>
+      <c r="L3" s="3" t="inlineStr">
+        <is>
+          <t>2023-11-26</t>
+        </is>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>没有</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>赵六</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
         <is>
           <t>15935702580</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="E4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="n"/>
+      <c r="G4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>第一批</t>
+        </is>
+      </c>
+      <c r="J4" s="4" t="inlineStr">
+        <is>
+          <t>2023-11-26</t>
+        </is>
+      </c>
+      <c r="K4" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="5" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="N4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" s="5" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>老七</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C5" s="2" t="n"/>
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>13935502580</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>7</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>小八</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>14935502580</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="E5" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="n"/>
+      <c r="G5" s="2" t="n"/>
+      <c r="H5" s="2" t="n"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>第一批</t>
+        </is>
+      </c>
+      <c r="J5" s="6" t="inlineStr">
+        <is>
+          <t>2023-11-27</t>
+        </is>
+      </c>
+      <c r="K5" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>第二批</t>
+        </is>
+      </c>
+      <c r="J6" s="6" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
+      <c r="K6" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>第三批</t>
+        </is>
+      </c>
+      <c r="J7" s="6" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
+      <c r="K7" s="6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="I8" t="inlineStr">
         <is>
-          <t>2023-11-26</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>2023-11-27</t>
-        </is>
+          <t>第四批</t>
+        </is>
+      </c>
+      <c r="J8" s="6" t="inlineStr">
+        <is>
+          <t>2024-01-29</t>
+        </is>
+      </c>
+      <c r="K8" s="6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="I9" t="inlineStr">
         <is>
-          <t>2023-11-27</t>
-        </is>
+          <t>第五批</t>
+        </is>
+      </c>
+      <c r="J9" s="6" t="inlineStr">
+        <is>
+          <t>2024-02-19</t>
+        </is>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="I10" t="inlineStr">
         <is>
+          <t>第六批</t>
+        </is>
+      </c>
+      <c r="J10" s="6" t="inlineStr">
+        <is>
+          <t>2024-03-11</t>
+        </is>
+      </c>
+      <c r="K10" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>小八</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n"/>
+      <c r="D11" s="1" t="inlineStr">
+        <is>
+          <t>14935502580</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1" t="n"/>
+      <c r="G11" s="1" t="n"/>
+      <c r="H11" s="1" t="n"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>第一批</t>
+        </is>
+      </c>
+      <c r="J11" s="4" t="inlineStr">
+        <is>
           <t>2023-11-27</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="5" t="inlineStr">
         <is>
           <t>2023-11-28</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>2023-12-18</t>
+      <c r="M11" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="N11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O11" s="5" t="inlineStr">
+        <is>
+          <t>不错</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="I12" t="inlineStr">
         <is>
-          <t>2024-01-08</t>
-        </is>
+          <t>第二批</t>
+        </is>
+      </c>
+      <c r="J12" s="4" t="inlineStr">
+        <is>
+          <t>2023-12-18</t>
+        </is>
+      </c>
+      <c r="K12" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="I13" t="inlineStr">
         <is>
-          <t>2024-01-29</t>
-        </is>
+          <t>第三批</t>
+        </is>
+      </c>
+      <c r="J13" s="4" t="inlineStr">
+        <is>
+          <t>2024-01-08</t>
+        </is>
+      </c>
+      <c r="K13" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="I14" t="inlineStr">
         <is>
-          <t>2024-02-19</t>
-        </is>
+          <t>第四批</t>
+        </is>
+      </c>
+      <c r="J14" s="4" t="inlineStr">
+        <is>
+          <t>2024-01-29</t>
+        </is>
+      </c>
+      <c r="K14" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="I15" t="inlineStr">
         <is>
+          <t>第五批</t>
+        </is>
+      </c>
+      <c r="J15" s="4" t="inlineStr">
+        <is>
+          <t>2024-02-19</t>
+        </is>
+      </c>
+      <c r="K15" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>第六批</t>
+        </is>
+      </c>
+      <c r="J16" s="4" t="inlineStr">
+        <is>
           <t>2024-03-11</t>
         </is>
       </c>
+      <c r="K16" s="4" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="40">
+    <mergeCell ref="A2"/>
+    <mergeCell ref="B2"/>
+    <mergeCell ref="C2"/>
+    <mergeCell ref="D2"/>
+    <mergeCell ref="E2"/>
+    <mergeCell ref="F2"/>
+    <mergeCell ref="G2"/>
+    <mergeCell ref="H2"/>
+    <mergeCell ref="A3"/>
+    <mergeCell ref="B3"/>
+    <mergeCell ref="C3"/>
+    <mergeCell ref="D3"/>
+    <mergeCell ref="E3"/>
+    <mergeCell ref="F3"/>
+    <mergeCell ref="G3"/>
+    <mergeCell ref="H3"/>
+    <mergeCell ref="A4"/>
+    <mergeCell ref="B4"/>
+    <mergeCell ref="C4"/>
+    <mergeCell ref="D4"/>
+    <mergeCell ref="E4"/>
+    <mergeCell ref="F4"/>
+    <mergeCell ref="G4"/>
+    <mergeCell ref="H4"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="D5:D10"/>
+    <mergeCell ref="E5:E10"/>
+    <mergeCell ref="F5:F10"/>
+    <mergeCell ref="G5:G10"/>
+    <mergeCell ref="H5:H10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="F11:F16"/>
+    <mergeCell ref="G11:G16"/>
+    <mergeCell ref="H11:H16"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>